<commit_message>
edited exemption calculation and no of files upload, updated database
</commit_message>
<xml_diff>
--- a/uploaded_files/examinable_staff_list.xlsx
+++ b/uploaded_files/examinable_staff_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\fyp\uploaded_files\Latest by Dr.Li\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\fyp\uploaded_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6B4A54-C0D5-4138-9191-5394C7693008}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04EB621-2C65-4226-97B2-B9679E186844}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="14730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,9 +276,6 @@
     <t>Svetlana Obraztsova (Lana)</t>
   </si>
   <si>
-    <t>Sourav SenGupta</t>
-  </si>
-  <si>
     <t>Yu Han</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
   </si>
   <si>
     <t>junzhao@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>Sourav Sen Gupta</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +623,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,6 +757,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1098,8 +1110,8 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1136,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>43</v>
@@ -1133,7 +1145,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1142,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>26</v>
@@ -1160,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>47</v>
@@ -1178,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>32</v>
@@ -1196,7 +1208,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>27</v>
@@ -1214,7 +1226,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>39</v>
@@ -1232,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>23</v>
@@ -1250,7 +1262,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>55</v>
@@ -1268,7 +1280,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>0</v>
@@ -1286,7 +1298,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
@@ -1304,7 +1316,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>2</v>
@@ -1322,7 +1334,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>48</v>
@@ -1340,7 +1352,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>3</v>
@@ -1358,7 +1370,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>68</v>
@@ -1376,7 +1388,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>28</v>
@@ -1394,10 +1406,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>54</v>
@@ -1412,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>29</v>
@@ -1430,7 +1442,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>4</v>
@@ -1448,7 +1460,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>33</v>
@@ -1466,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>5</v>
@@ -1484,7 +1496,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>70</v>
@@ -1502,7 +1514,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>6</v>
@@ -1520,7 +1532,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>7</v>
@@ -1538,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>8</v>
@@ -1556,7 +1568,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>30</v>
@@ -1574,7 +1586,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>34</v>
@@ -1592,7 +1604,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>49</v>
@@ -1610,7 +1622,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>9</v>
@@ -1628,7 +1640,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>40</v>
@@ -1646,7 +1658,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>25</v>
@@ -1664,7 +1676,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>50</v>
@@ -1682,9 +1694,9 @@
         <v>31</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -1700,7 +1712,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>51</v>
@@ -1718,10 +1730,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>54</v>
@@ -1736,7 +1748,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>67</v>
@@ -1754,7 +1766,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>10</v>
@@ -1772,7 +1784,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>72</v>
@@ -1790,7 +1802,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>38</v>
@@ -1808,7 +1820,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>11</v>
@@ -1826,7 +1838,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>77</v>
@@ -1844,7 +1856,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>24</v>
@@ -1862,10 +1874,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>59</v>
@@ -1880,10 +1892,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>54</v>
@@ -1898,13 +1910,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="E45" s="26">
         <v>0.5</v>
@@ -1916,7 +1928,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>73</v>
@@ -1934,7 +1946,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>12</v>
@@ -1952,7 +1964,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>74</v>
@@ -1970,7 +1982,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>76</v>
@@ -1988,7 +2000,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>13</v>
@@ -2006,7 +2018,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>35</v>
@@ -2024,7 +2036,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>36</v>
@@ -2042,7 +2054,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>57</v>
@@ -2060,7 +2072,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>14</v>
@@ -2078,7 +2090,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>15</v>
@@ -2096,7 +2108,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>16</v>
@@ -2114,7 +2126,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>75</v>
@@ -2133,7 +2145,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>79</v>
@@ -2151,7 +2163,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>65</v>
@@ -2169,7 +2181,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>61</v>
@@ -2188,7 +2200,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>52</v>
@@ -2206,10 +2218,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>82</v>
+        <v>171</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>59</v>
@@ -2224,7 +2236,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>17</v>
@@ -2242,7 +2254,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>62</v>
@@ -2260,9 +2272,9 @@
         <v>63</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="C65" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="34" t="s">
         <v>81</v>
       </c>
       <c r="D65" s="14" t="s">
@@ -2278,7 +2290,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>60</v>
@@ -2297,7 +2309,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>53</v>
@@ -2315,7 +2327,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>18</v>
@@ -2333,7 +2345,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>41</v>
@@ -2351,7 +2363,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>19</v>
@@ -2369,7 +2381,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>31</v>
@@ -2387,10 +2399,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D72" s="22" t="s">
         <v>46</v>
@@ -2405,7 +2417,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>69</v>
@@ -2423,7 +2435,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>20</v>
@@ -2441,10 +2453,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D75" s="13" t="s">
         <v>56</v>
@@ -2459,7 +2471,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>80</v>
@@ -2477,7 +2489,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>21</v>
@@ -2495,10 +2507,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D78" s="13" t="s">
         <v>54</v>
@@ -2513,7 +2525,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>22</v>
@@ -2531,7 +2543,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>71</v>

</xml_diff>